<commit_message>
Update academic schedule templates: Revised formatting and structure for improved clarity and usability.
</commit_message>
<xml_diff>
--- a/public/templates/academic_schedules_pontisis.xlsx
+++ b/public/templates/academic_schedules_pontisis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\dev\pontiapp-laravel\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E0E03B-3DAB-4484-85C5-3E83857F4B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBFE589-1C06-4C12-989B-55E60C4300BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="153">
   <si>
     <t>Prog. Academico</t>
   </si>
@@ -556,6 +556,15 @@
   </si>
   <si>
     <t>Aula Nombre</t>
+  </si>
+  <si>
+    <t>Curso Nombre</t>
+  </si>
+  <si>
+    <t>Docente Nombre</t>
+  </si>
+  <si>
+    <t>Pabellon Nombre</t>
   </si>
 </sst>
 </file>
@@ -580,7 +589,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +612,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4F81BD"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -633,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -645,6 +660,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -950,30 +969,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="34.7109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="7"/>
+    <col min="16" max="16" width="26.140625" customWidth="1"/>
+    <col min="17" max="17" width="26.85546875" customWidth="1"/>
+    <col min="18" max="18" width="15" style="7" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1017,9 +1042,15 @@
         <v>148</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>149</v>
       </c>
     </row>

</xml_diff>